<commit_message>
CSV and Excel files added.
</commit_message>
<xml_diff>
--- a/amazon-product-reviews/Apple Magic Mouse (Technology) - Amazon Product Reviews.xlsx
+++ b/amazon-product-reviews/Apple Magic Mouse (Technology) - Amazon Product Reviews.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mesrurebeybinesen/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/Projects/nlp-datasets/amazon-product-reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893744A6-6BFA-6245-8C3D-2EEF34DAABB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D47D1F-444E-B04A-AF37-30674DA222FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="275">
   <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> urls</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Good Example of Form Over Function I think this is possibly the worst designed product Apple has ever made, in my opinion. I see it as putting form well above function. It was like Apple decided to combine a mouse with a trackpad. In this case, the tracking is done by moving the trackpad around as opposed to using the pad to track. If I remember correctly, someone else on here referred to this mouse as an ergonomic disaster and I have to agree. The sides of this mouse are sharp and pinching with barely anything to grab on to. It appears the mouse was not designed with a consideration for where to put thumbs and any other fingers people might need to use to hold on to a mouse, or at least a spot where they can rest those fingers so they're not in the way . What's more, if my thumb drops as it is inclined to do due to gravity and because it is in pursuit of a stronger grip then my thumb gets pinched between the silver base and the white top part of the mouse that functions like a giant mouse button . It's like my thumb is in the way of this mouse doing what it wants to do. On the opposite side, my little finger gets dragged and pushed around on the mousepad as it has no place to go. To make matters worse, the white touch surface top does not feel secure. It rocks sideways ever so slightly. That loose top gets tiring after a while and I think it may be in part responsible for my struggles getting the mouse to start selecting text on the letter that I want it to start selecting on. The flat white surface of the mouse, the mini trackpad that doesn't track, is good for quick scrolling but there's a catch, I find it gets tiring after a while because my pointer finger is repeatedly hitting and gliding over a hard surface. Sometimes my fingernail scrapes along the surface as well. It was after my fingernail got caught scraping the top of the mouse while scrolling one day that led me to say to myself enough, I'm not using this anymore. In addition to the scrolling getting tired after a while, my index finger does drift over to the middle of the mouse. Having used ergonomic mice, I now believe that the flat shape is partly responsible because there is so little for my hand to grip on to. The drifting leads left clicks to turn into right clicks. It is annoying when I occasionally click on something expecting to select it or what not, only to see the context menu pop up instead. I also got this mouse for my mother to use and her finger drifts over to the right so often that I decided to turn off the right click function to help her out. She doesn't use the right click button so she isn't missing anything but others might have use for the right click button. Despite that, the scrolling feature gets in her way still and she uses that. Another issue both of us have with scrolling, and this is one of the most annoying things about this mouse, is that we often, her more than me I think, find ourselves scrolling sideways while scrolling down or up when we just want to scroll down or up. I've never had that issue on mice with scroll wheels, or any other mouse for that matter. There'd be times when I'd have what I'm looking at lined up just right and then when I scroll, I can't scroll down or up in a straight line with out it moving sideways at some point. Another annoying thing about the touch surface of the mouse is that occasionally I'll brush it with my finger when I'm in the process of putting my hand back on to the mouse after typing on the keyboard. That leads to something happening that I didn't want which needs to then be corrected. One of the bonuses of the touch surface is that it opens the door for tapping and swiping, adding functionality without the need for buttons. I never got comfortable with swiping on a mouse, while I just used tapping in order to use Mission Control. The way it is set up requires a double two-finger tap on the touch surface but what feels like half the time, I don't tap the top of the mouse right and I have to do it again until I get Mission Control to work . That issue didn't go away over time with practice. Tapping, for me, is not a replacement for a third button on a traditional mouse. Another negative, and this one is talked about a lot, is that the lightning port used for recharging is on the underside of the mouse which means in order to recharge the mouse it has to be on its side or laying down with its belly up. That of course means you can't recharge the mouse and use it at the same time. To make matters worse, there aren't many positives I find with this mouse. It is Apple's mouse, for one, and for that you are assured lasting compatibility with Macs. I've had multiple experiences where Logitech mice all of a sudden don't work properly or are not compatible after an update or with a new Mac. Two, the battery lasts a good amount of time. Maybe up to three months on a single charge. That seems good to me. However, I did encounter an issue when I recharged the mouse the first time. Despite following the directions on how to check when the mouse is fully charged, when I went to use it again the following morning I noticed that the charge was at 74%. It was at 12% before I recharged it the night before and said it was at 100% when I unplugged it. I had to recharge it a second time in order to get it up to 100%. Hopefully, that was just a one time issue. The third positive is that the mouse is lightweight. I prefer lightweight mice but in this case, it doesn't make up for the drawbacks. The fourth positive is that its shape and weight makes it easy to fit in a bag or in a pocket. In the end, the positives do not come close to outweighing its negatives for me. The key phrase is, "for me," as there are people out there that prefer tapping and swiping and smaller mice. From my experience, seeing my mother's struggles and reading other reviews, this mouse is simply not for everyone and I don't fully understand why Apple designed it the way they did. Too much form over function to me. I would take a corded mouse over this one if I had to. Unless you prefer mice like the Apple Magic Mouse as opposed to a traditional style mouse with scroll wheels and a mouse like shape, I'd recommend trying out other mice first before paying for this one. Chances are you'll find something that's more comfortable and less frustrating to use for less money. But if you are willing to spend a bit more. Then there are mice out there like the Logitech MX Master which are designed to be more comfortable, may even feel like they are better made than the Magic Mouse, while having more features and capabilities.</t>
   </si>
   <si>
@@ -858,6 +852,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Url</t>
   </si>
 </sst>
 </file>
@@ -1243,9 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1255,21 +1253,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
         <v>44927</v>
@@ -1277,10 +1275,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
         <v>44927</v>
@@ -1288,10 +1286,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
         <v>44927</v>
@@ -1299,10 +1297,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
         <v>44927</v>
@@ -1310,10 +1308,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
         <v>44927</v>
@@ -1321,10 +1319,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
         <v>44927</v>
@@ -1332,10 +1330,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
         <v>44927</v>
@@ -1343,10 +1341,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
         <v>44927</v>
@@ -1354,10 +1352,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
         <v>44927</v>
@@ -1365,10 +1363,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
         <v>44928</v>
@@ -1376,10 +1374,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
         <v>44928</v>
@@ -1387,10 +1385,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
         <v>44928</v>
@@ -1398,10 +1396,10 @@
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5">
         <v>44928</v>
@@ -1409,10 +1407,10 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
         <v>44928</v>
@@ -1420,10 +1418,10 @@
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5">
         <v>44928</v>
@@ -1431,10 +1429,10 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
         <v>44928</v>
@@ -1442,10 +1440,10 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
         <v>44928</v>
@@ -1453,10 +1451,10 @@
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
         <v>44928</v>
@@ -1464,10 +1462,10 @@
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5">
         <v>44928</v>
@@ -1475,10 +1473,10 @@
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
         <v>44928</v>
@@ -1486,10 +1484,10 @@
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5">
         <v>44928</v>
@@ -1497,10 +1495,10 @@
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
         <v>44929</v>
@@ -1508,10 +1506,10 @@
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="5">
         <v>44929</v>
@@ -1519,10 +1517,10 @@
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
         <v>44929</v>
@@ -1530,10 +1528,10 @@
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" s="5">
         <v>44929</v>
@@ -1541,10 +1539,10 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>44929</v>
@@ -1552,10 +1550,10 @@
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="5">
         <v>44929</v>
@@ -1563,10 +1561,10 @@
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" s="5">
         <v>44929</v>
@@ -1574,10 +1572,10 @@
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" s="5">
         <v>44929</v>
@@ -1585,10 +1583,10 @@
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="5">
         <v>44929</v>
@@ -1596,10 +1594,10 @@
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C32" s="5">
         <v>44929</v>
@@ -1607,10 +1605,10 @@
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" s="5">
         <v>44929</v>
@@ -1618,10 +1616,10 @@
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" s="5">
         <v>44929</v>
@@ -1629,10 +1627,10 @@
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5">
         <v>44929</v>
@@ -1640,10 +1638,10 @@
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C36" s="5">
         <v>44929</v>
@@ -1651,10 +1649,10 @@
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="5">
         <v>44929</v>
@@ -1662,10 +1660,10 @@
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" s="5">
         <v>44929</v>
@@ -1673,10 +1671,10 @@
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39" s="5">
         <v>44929</v>
@@ -1684,10 +1682,10 @@
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="5">
         <v>44929</v>
@@ -1695,10 +1693,10 @@
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C41" s="5">
         <v>44929</v>
@@ -1706,10 +1704,10 @@
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5">
         <v>44929</v>
@@ -1717,10 +1715,10 @@
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" s="5">
         <v>44929</v>
@@ -1728,10 +1726,10 @@
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5">
         <v>44929</v>
@@ -1739,10 +1737,10 @@
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" s="5">
         <v>44929</v>
@@ -1750,10 +1748,10 @@
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" s="5">
         <v>44929</v>
@@ -1761,10 +1759,10 @@
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C47" s="5">
         <v>44930</v>
@@ -1772,10 +1770,10 @@
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48" s="5">
         <v>44930</v>
@@ -1783,10 +1781,10 @@
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" s="5">
         <v>44930</v>
@@ -1794,10 +1792,10 @@
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" s="5">
         <v>44930</v>
@@ -1805,10 +1803,10 @@
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" s="5">
         <v>44930</v>
@@ -1816,10 +1814,10 @@
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" s="5">
         <v>44930</v>
@@ -1827,10 +1825,10 @@
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" s="5">
         <v>44930</v>
@@ -1838,10 +1836,10 @@
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="5">
         <v>44930</v>
@@ -1849,10 +1847,10 @@
     </row>
     <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" s="5">
         <v>44930</v>
@@ -1860,10 +1858,10 @@
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" s="5">
         <v>44930</v>
@@ -1871,10 +1869,10 @@
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" s="5">
         <v>44930</v>
@@ -1882,10 +1880,10 @@
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" s="5">
         <v>44930</v>
@@ -1893,10 +1891,10 @@
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C59" s="5">
         <v>44930</v>
@@ -1904,10 +1902,10 @@
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="5">
         <v>44930</v>
@@ -1915,10 +1913,10 @@
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C61" s="5">
         <v>44930</v>
@@ -1926,10 +1924,10 @@
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62" s="5">
         <v>44930</v>
@@ -1937,10 +1935,10 @@
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63" s="5">
         <v>44930</v>
@@ -1948,10 +1946,10 @@
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C64" s="5">
         <v>44930</v>
@@ -1959,10 +1957,10 @@
     </row>
     <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65" s="5">
         <v>44931</v>
@@ -1970,10 +1968,10 @@
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" s="5">
         <v>44931</v>
@@ -1981,10 +1979,10 @@
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" s="5">
         <v>44931</v>
@@ -1992,10 +1990,10 @@
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68" s="5">
         <v>44931</v>
@@ -2003,10 +2001,10 @@
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" s="5">
         <v>44931</v>
@@ -2014,10 +2012,10 @@
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70" s="5">
         <v>44931</v>
@@ -2025,10 +2023,10 @@
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" s="5">
         <v>44931</v>
@@ -2036,10 +2034,10 @@
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72" s="5">
         <v>44931</v>
@@ -2047,10 +2045,10 @@
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C73" s="5">
         <v>44931</v>
@@ -2058,10 +2056,10 @@
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C74" s="5">
         <v>44931</v>
@@ -2069,10 +2067,10 @@
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75" s="5">
         <v>44931</v>
@@ -2080,10 +2078,10 @@
     </row>
     <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C76" s="5">
         <v>44931</v>
@@ -2091,10 +2089,10 @@
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C77" s="5">
         <v>44931</v>
@@ -2102,10 +2100,10 @@
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C78" s="5">
         <v>44931</v>
@@ -2113,10 +2111,10 @@
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C79" s="5">
         <v>44931</v>
@@ -2124,10 +2122,10 @@
     </row>
     <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C80" s="5">
         <v>44931</v>
@@ -2135,10 +2133,10 @@
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C81" s="5">
         <v>44931</v>
@@ -2146,10 +2144,10 @@
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C82" s="5">
         <v>44931</v>
@@ -2157,10 +2155,10 @@
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83" s="5">
         <v>44931</v>
@@ -2168,10 +2166,10 @@
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C84" s="5">
         <v>44931</v>
@@ -2179,10 +2177,10 @@
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C85" s="5">
         <v>44931</v>
@@ -2190,10 +2188,10 @@
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" s="5">
         <v>44931</v>
@@ -2201,10 +2199,10 @@
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C87" s="5">
         <v>44931</v>
@@ -2212,10 +2210,10 @@
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C88" s="5">
         <v>44931</v>
@@ -2223,10 +2221,10 @@
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C89" s="5">
         <v>44931</v>
@@ -2234,10 +2232,10 @@
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C90" s="5">
         <v>44931</v>
@@ -2245,10 +2243,10 @@
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C91" s="5">
         <v>44931</v>
@@ -2256,10 +2254,10 @@
     </row>
     <row r="92" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92" s="5">
         <v>44931</v>
@@ -2267,10 +2265,10 @@
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C93" s="5">
         <v>44931</v>
@@ -2278,10 +2276,10 @@
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C94" s="5">
         <v>44931</v>
@@ -2289,10 +2287,10 @@
     </row>
     <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C95" s="5">
         <v>44931</v>
@@ -2300,10 +2298,10 @@
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C96" s="5">
         <v>44931</v>
@@ -2311,10 +2309,10 @@
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C97" s="5">
         <v>44931</v>
@@ -2322,10 +2320,10 @@
     </row>
     <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C98" s="5">
         <v>44931</v>
@@ -2333,10 +2331,10 @@
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C99" s="5">
         <v>44931</v>
@@ -2344,10 +2342,10 @@
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C100" s="5">
         <v>44931</v>
@@ -2355,10 +2353,10 @@
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C101" s="5">
         <v>44931</v>
@@ -2366,10 +2364,10 @@
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C102" s="5">
         <v>44931</v>
@@ -2377,10 +2375,10 @@
     </row>
     <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C103" s="5">
         <v>44931</v>
@@ -2388,10 +2386,10 @@
     </row>
     <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C104" s="5">
         <v>44931</v>
@@ -2399,10 +2397,10 @@
     </row>
     <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C105" s="5">
         <v>44931</v>
@@ -2410,10 +2408,10 @@
     </row>
     <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C106" s="5">
         <v>44931</v>
@@ -2421,10 +2419,10 @@
     </row>
     <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C107" s="5">
         <v>44931</v>
@@ -2432,10 +2430,10 @@
     </row>
     <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C108" s="5">
         <v>44931</v>
@@ -2443,10 +2441,10 @@
     </row>
     <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C109" s="5">
         <v>44931</v>
@@ -2454,10 +2452,10 @@
     </row>
     <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C110" s="5">
         <v>44931</v>
@@ -2465,10 +2463,10 @@
     </row>
     <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C111" s="5">
         <v>44931</v>
@@ -2476,10 +2474,10 @@
     </row>
     <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C112" s="5">
         <v>44931</v>
@@ -2487,10 +2485,10 @@
     </row>
     <row r="113" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C113" s="5">
         <v>44931</v>
@@ -2498,10 +2496,10 @@
     </row>
     <row r="114" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C114" s="5">
         <v>44931</v>
@@ -2509,10 +2507,10 @@
     </row>
     <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C115" s="5">
         <v>44931</v>
@@ -2520,10 +2518,10 @@
     </row>
     <row r="116" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C116" s="5">
         <v>44931</v>
@@ -2531,10 +2529,10 @@
     </row>
     <row r="117" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C117" s="5">
         <v>44931</v>
@@ -2542,10 +2540,10 @@
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C118" s="5">
         <v>44931</v>
@@ -2553,10 +2551,10 @@
     </row>
     <row r="119" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C119" s="5">
         <v>44931</v>
@@ -2564,10 +2562,10 @@
     </row>
     <row r="120" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C120" s="5">
         <v>44931</v>
@@ -2575,10 +2573,10 @@
     </row>
     <row r="121" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C121" s="5">
         <v>44931</v>
@@ -2586,10 +2584,10 @@
     </row>
     <row r="122" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C122" s="5">
         <v>44932</v>
@@ -2597,10 +2595,10 @@
     </row>
     <row r="123" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C123" s="5">
         <v>44932</v>
@@ -2608,10 +2606,10 @@
     </row>
     <row r="124" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C124" s="5">
         <v>44932</v>
@@ -2619,10 +2617,10 @@
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C125" s="5">
         <v>44932</v>
@@ -2630,10 +2628,10 @@
     </row>
     <row r="126" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C126" s="5">
         <v>44932</v>
@@ -2641,10 +2639,10 @@
     </row>
     <row r="127" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C127" s="5">
         <v>44932</v>
@@ -2652,10 +2650,10 @@
     </row>
     <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C128" s="5">
         <v>44932</v>
@@ -2663,10 +2661,10 @@
     </row>
     <row r="129" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C129" s="5">
         <v>44932</v>
@@ -2674,10 +2672,10 @@
     </row>
     <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C130" s="5">
         <v>44932</v>
@@ -2685,10 +2683,10 @@
     </row>
     <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C131" s="5">
         <v>44932</v>
@@ -2696,10 +2694,10 @@
     </row>
     <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C132" s="5">
         <v>44932</v>
@@ -2707,10 +2705,10 @@
     </row>
     <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C133" s="5">
         <v>44932</v>
@@ -2718,10 +2716,10 @@
     </row>
     <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C134" s="5">
         <v>44932</v>
@@ -2729,10 +2727,10 @@
     </row>
     <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C135" s="5">
         <v>44932</v>
@@ -2740,10 +2738,10 @@
     </row>
     <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C136" s="5">
         <v>44932</v>
@@ -2751,10 +2749,10 @@
     </row>
     <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C137" s="5">
         <v>44932</v>
@@ -2762,10 +2760,10 @@
     </row>
     <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C138" s="5">
         <v>44932</v>
@@ -2773,10 +2771,10 @@
     </row>
     <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C139" s="5">
         <v>44932</v>
@@ -2784,10 +2782,10 @@
     </row>
     <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C140" s="5">
         <v>44932</v>
@@ -2795,10 +2793,10 @@
     </row>
     <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C141" s="5">
         <v>44932</v>
@@ -2806,10 +2804,10 @@
     </row>
     <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C142" s="5">
         <v>44932</v>
@@ -2817,10 +2815,10 @@
     </row>
     <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C143" s="5">
         <v>44932</v>
@@ -2828,10 +2826,10 @@
     </row>
     <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C144" s="5">
         <v>44932</v>
@@ -2839,10 +2837,10 @@
     </row>
     <row r="145" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C145" s="5">
         <v>44932</v>
@@ -2850,10 +2848,10 @@
     </row>
     <row r="146" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C146" s="5">
         <v>44932</v>
@@ -2861,10 +2859,10 @@
     </row>
     <row r="147" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C147" s="5">
         <v>44932</v>
@@ -2872,10 +2870,10 @@
     </row>
     <row r="148" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C148" s="5">
         <v>44932</v>
@@ -2883,10 +2881,10 @@
     </row>
     <row r="149" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C149" s="5">
         <v>44932</v>
@@ -2894,10 +2892,10 @@
     </row>
     <row r="150" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C150" s="5">
         <v>44932</v>
@@ -2905,10 +2903,10 @@
     </row>
     <row r="151" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C151" s="5">
         <v>44932</v>
@@ -2916,10 +2914,10 @@
     </row>
     <row r="152" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C152" s="5">
         <v>44932</v>
@@ -2927,10 +2925,10 @@
     </row>
     <row r="153" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C153" s="5">
         <v>44932</v>
@@ -2938,10 +2936,10 @@
     </row>
     <row r="154" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C154" s="5">
         <v>44932</v>
@@ -2949,10 +2947,10 @@
     </row>
     <row r="155" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C155" s="5">
         <v>44932</v>
@@ -2960,10 +2958,10 @@
     </row>
     <row r="156" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C156" s="5">
         <v>44932</v>
@@ -2971,10 +2969,10 @@
     </row>
     <row r="157" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C157" s="5">
         <v>44933</v>
@@ -2982,10 +2980,10 @@
     </row>
     <row r="158" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C158" s="5">
         <v>44933</v>
@@ -2993,10 +2991,10 @@
     </row>
     <row r="159" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C159" s="5">
         <v>44933</v>
@@ -3004,10 +3002,10 @@
     </row>
     <row r="160" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C160" s="5">
         <v>44933</v>
@@ -3015,10 +3013,10 @@
     </row>
     <row r="161" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C161" s="5">
         <v>44933</v>
@@ -3026,10 +3024,10 @@
     </row>
     <row r="162" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C162" s="5">
         <v>44933</v>
@@ -3037,10 +3035,10 @@
     </row>
     <row r="163" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C163" s="5">
         <v>44933</v>
@@ -3048,10 +3046,10 @@
     </row>
     <row r="164" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C164" s="5">
         <v>44933</v>
@@ -3059,10 +3057,10 @@
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C165" s="5">
         <v>44933</v>
@@ -3070,10 +3068,10 @@
     </row>
     <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C166" s="5">
         <v>44933</v>
@@ -3081,10 +3079,10 @@
     </row>
     <row r="167" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C167" s="5">
         <v>44933</v>
@@ -3092,10 +3090,10 @@
     </row>
     <row r="168" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C168" s="5">
         <v>44933</v>
@@ -3103,10 +3101,10 @@
     </row>
     <row r="169" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C169" s="5">
         <v>44933</v>
@@ -3114,10 +3112,10 @@
     </row>
     <row r="170" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C170" s="5">
         <v>44933</v>
@@ -3125,10 +3123,10 @@
     </row>
     <row r="171" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C171" s="5">
         <v>44933</v>
@@ -3136,10 +3134,10 @@
     </row>
     <row r="172" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C172" s="5">
         <v>44933</v>
@@ -3147,10 +3145,10 @@
     </row>
     <row r="173" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C173" s="5">
         <v>44933</v>
@@ -3158,10 +3156,10 @@
     </row>
     <row r="174" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C174" s="5">
         <v>44933</v>
@@ -3169,10 +3167,10 @@
     </row>
     <row r="175" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C175" s="5">
         <v>44933</v>
@@ -3180,10 +3178,10 @@
     </row>
     <row r="176" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C176" s="5">
         <v>44933</v>
@@ -3191,10 +3189,10 @@
     </row>
     <row r="177" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C177" s="5">
         <v>44933</v>
@@ -3202,10 +3200,10 @@
     </row>
     <row r="178" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C178" s="5">
         <v>44933</v>
@@ -3213,10 +3211,10 @@
     </row>
     <row r="179" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C179" s="5">
         <v>44933</v>
@@ -3224,10 +3222,10 @@
     </row>
     <row r="180" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C180" s="5">
         <v>44933</v>
@@ -3235,10 +3233,10 @@
     </row>
     <row r="181" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C181" s="5">
         <v>44933</v>
@@ -3246,10 +3244,10 @@
     </row>
     <row r="182" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C182" s="5">
         <v>44933</v>
@@ -3257,10 +3255,10 @@
     </row>
     <row r="183" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C183" s="5">
         <v>44933</v>
@@ -3268,10 +3266,10 @@
     </row>
     <row r="184" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C184" s="5">
         <v>44933</v>
@@ -3279,10 +3277,10 @@
     </row>
     <row r="185" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C185" s="5">
         <v>44933</v>
@@ -3290,10 +3288,10 @@
     </row>
     <row r="186" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C186" s="5">
         <v>44933</v>
@@ -3301,10 +3299,10 @@
     </row>
     <row r="187" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C187" s="5">
         <v>44933</v>
@@ -3312,10 +3310,10 @@
     </row>
     <row r="188" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C188" s="5">
         <v>44933</v>
@@ -3323,10 +3321,10 @@
     </row>
     <row r="189" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C189" s="5">
         <v>44933</v>
@@ -3334,10 +3332,10 @@
     </row>
     <row r="190" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C190" s="5">
         <v>44933</v>
@@ -3345,10 +3343,10 @@
     </row>
     <row r="191" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C191" s="5">
         <v>44933</v>
@@ -3356,10 +3354,10 @@
     </row>
     <row r="192" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C192" s="5">
         <v>44933</v>
@@ -3367,10 +3365,10 @@
     </row>
     <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C193" s="5">
         <v>44933</v>
@@ -3378,10 +3376,10 @@
     </row>
     <row r="194" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C194" s="5">
         <v>44933</v>
@@ -3389,10 +3387,10 @@
     </row>
     <row r="195" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C195" s="5">
         <v>44933</v>
@@ -3400,10 +3398,10 @@
     </row>
     <row r="196" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C196" s="5">
         <v>44933</v>
@@ -3411,10 +3409,10 @@
     </row>
     <row r="197" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C197" s="5">
         <v>44933</v>
@@ -3422,10 +3420,10 @@
     </row>
     <row r="198" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C198" s="5">
         <v>44933</v>
@@ -3433,10 +3431,10 @@
     </row>
     <row r="199" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C199" s="5">
         <v>44933</v>
@@ -3444,10 +3442,10 @@
     </row>
     <row r="200" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C200" s="5">
         <v>44933</v>
@@ -3455,10 +3453,10 @@
     </row>
     <row r="201" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C201" s="5">
         <v>44933</v>
@@ -3466,10 +3464,10 @@
     </row>
     <row r="202" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C202" s="5">
         <v>44933</v>
@@ -3477,10 +3475,10 @@
     </row>
     <row r="203" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C203" s="5">
         <v>44933</v>
@@ -3488,10 +3486,10 @@
     </row>
     <row r="204" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C204" s="5">
         <v>44933</v>
@@ -3499,10 +3497,10 @@
     </row>
     <row r="205" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C205" s="5">
         <v>44933</v>
@@ -3510,10 +3508,10 @@
     </row>
     <row r="206" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C206" s="5">
         <v>44933</v>
@@ -3521,10 +3519,10 @@
     </row>
     <row r="207" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C207" s="5">
         <v>44933</v>
@@ -3532,10 +3530,10 @@
     </row>
     <row r="208" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C208" s="5">
         <v>44933</v>
@@ -3543,10 +3541,10 @@
     </row>
     <row r="209" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C209" s="5">
         <v>44933</v>
@@ -3554,10 +3552,10 @@
     </row>
     <row r="210" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C210" s="5">
         <v>44933</v>
@@ -3565,10 +3563,10 @@
     </row>
     <row r="211" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C211" s="5">
         <v>44933</v>
@@ -3576,10 +3574,10 @@
     </row>
     <row r="212" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C212" s="5">
         <v>44933</v>
@@ -3587,10 +3585,10 @@
     </row>
     <row r="213" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C213" s="5">
         <v>44933</v>
@@ -3598,10 +3596,10 @@
     </row>
     <row r="214" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C214" s="5">
         <v>44933</v>
@@ -3609,10 +3607,10 @@
     </row>
     <row r="215" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C215" s="5">
         <v>44933</v>
@@ -3620,10 +3618,10 @@
     </row>
     <row r="216" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C216" s="5">
         <v>44933</v>
@@ -3631,10 +3629,10 @@
     </row>
     <row r="217" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C217" s="5">
         <v>44933</v>
@@ -3642,10 +3640,10 @@
     </row>
     <row r="218" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C218" s="5">
         <v>44933</v>
@@ -3653,10 +3651,10 @@
     </row>
     <row r="219" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C219" s="5">
         <v>44933</v>
@@ -3664,10 +3662,10 @@
     </row>
     <row r="220" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C220" s="5">
         <v>44933</v>
@@ -3675,10 +3673,10 @@
     </row>
     <row r="221" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C221" s="5">
         <v>44933</v>
@@ -3686,10 +3684,10 @@
     </row>
     <row r="222" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C222" s="5">
         <v>44933</v>
@@ -3697,10 +3695,10 @@
     </row>
     <row r="223" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C223" s="5">
         <v>44933</v>
@@ -3708,10 +3706,10 @@
     </row>
     <row r="224" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C224" s="5">
         <v>44933</v>
@@ -3719,10 +3717,10 @@
     </row>
     <row r="225" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C225" s="5">
         <v>44933</v>
@@ -3730,10 +3728,10 @@
     </row>
     <row r="226" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C226" s="5">
         <v>44933</v>
@@ -3741,10 +3739,10 @@
     </row>
     <row r="227" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C227" s="5">
         <v>44933</v>
@@ -3752,10 +3750,10 @@
     </row>
     <row r="228" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C228" s="5">
         <v>44933</v>
@@ -3763,10 +3761,10 @@
     </row>
     <row r="229" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C229" s="5">
         <v>44933</v>
@@ -3774,10 +3772,10 @@
     </row>
     <row r="230" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C230" s="5">
         <v>44933</v>
@@ -3785,10 +3783,10 @@
     </row>
     <row r="231" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C231" s="5">
         <v>44933</v>
@@ -3796,10 +3794,10 @@
     </row>
     <row r="232" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C232" s="5">
         <v>44933</v>
@@ -3807,10 +3805,10 @@
     </row>
     <row r="233" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C233" s="5">
         <v>44933</v>
@@ -3818,10 +3816,10 @@
     </row>
     <row r="234" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C234" s="5">
         <v>44933</v>
@@ -3829,10 +3827,10 @@
     </row>
     <row r="235" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C235" s="5">
         <v>44933</v>
@@ -3840,10 +3838,10 @@
     </row>
     <row r="236" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C236" s="5">
         <v>44933</v>
@@ -3851,10 +3849,10 @@
     </row>
     <row r="237" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C237" s="5">
         <v>44933</v>
@@ -3862,10 +3860,10 @@
     </row>
     <row r="238" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C238" s="5">
         <v>44934</v>
@@ -3873,10 +3871,10 @@
     </row>
     <row r="239" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C239" s="5">
         <v>44934</v>
@@ -3884,10 +3882,10 @@
     </row>
     <row r="240" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C240" s="5">
         <v>44934</v>
@@ -3895,10 +3893,10 @@
     </row>
     <row r="241" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C241" s="5">
         <v>44934</v>
@@ -3906,10 +3904,10 @@
     </row>
     <row r="242" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C242" s="5">
         <v>44934</v>
@@ -3917,10 +3915,10 @@
     </row>
     <row r="243" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C243" s="5">
         <v>44934</v>
@@ -3928,10 +3926,10 @@
     </row>
     <row r="244" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C244" s="5">
         <v>44934</v>
@@ -3939,10 +3937,10 @@
     </row>
     <row r="245" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C245" s="5">
         <v>44934</v>
@@ -3950,10 +3948,10 @@
     </row>
     <row r="246" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C246" s="5">
         <v>44934</v>
@@ -3961,10 +3959,10 @@
     </row>
     <row r="247" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C247" s="5">
         <v>44934</v>
@@ -3972,10 +3970,10 @@
     </row>
     <row r="248" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C248" s="5">
         <v>44934</v>
@@ -3983,10 +3981,10 @@
     </row>
     <row r="249" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C249" s="5">
         <v>44934</v>
@@ -3994,10 +3992,10 @@
     </row>
     <row r="250" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C250" s="5">
         <v>44934</v>
@@ -4005,10 +4003,10 @@
     </row>
     <row r="251" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C251" s="5">
         <v>44934</v>
@@ -4016,10 +4014,10 @@
     </row>
     <row r="252" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C252" s="5">
         <v>44934</v>
@@ -4027,10 +4025,10 @@
     </row>
     <row r="253" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C253" s="5">
         <v>44934</v>
@@ -4038,10 +4036,10 @@
     </row>
     <row r="254" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C254" s="5">
         <v>44934</v>
@@ -4049,10 +4047,10 @@
     </row>
     <row r="255" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C255" s="5">
         <v>44934</v>
@@ -4060,10 +4058,10 @@
     </row>
     <row r="256" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C256" s="5">
         <v>44934</v>
@@ -4071,10 +4069,10 @@
     </row>
     <row r="257" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C257" s="5">
         <v>44934</v>
@@ -4082,10 +4080,10 @@
     </row>
     <row r="258" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C258" s="5">
         <v>44934</v>
@@ -4093,10 +4091,10 @@
     </row>
     <row r="259" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C259" s="5">
         <v>44934</v>
@@ -4104,10 +4102,10 @@
     </row>
     <row r="260" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C260" s="5">
         <v>44934</v>
@@ -4115,10 +4113,10 @@
     </row>
     <row r="261" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C261" s="5">
         <v>44934</v>
@@ -4126,10 +4124,10 @@
     </row>
     <row r="262" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C262" s="5">
         <v>44934</v>
@@ -4137,10 +4135,10 @@
     </row>
     <row r="263" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C263" s="5">
         <v>44934</v>
@@ -4148,10 +4146,10 @@
     </row>
     <row r="264" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C264" s="5">
         <v>44934</v>
@@ -4159,10 +4157,10 @@
     </row>
     <row r="265" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C265" s="5">
         <v>44934</v>
@@ -4170,10 +4168,10 @@
     </row>
     <row r="266" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C266" s="5">
         <v>44934</v>
@@ -4181,10 +4179,10 @@
     </row>
     <row r="267" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C267" s="5">
         <v>44934</v>
@@ -4192,10 +4190,10 @@
     </row>
     <row r="268" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C268" s="5">
         <v>44934</v>
@@ -4203,10 +4201,10 @@
     </row>
     <row r="269" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C269" s="5">
         <v>44934</v>
@@ -4214,10 +4212,10 @@
     </row>
     <row r="270" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C270" s="5">
         <v>44934</v>
@@ -4225,10 +4223,10 @@
     </row>
     <row r="271" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C271" s="5">
         <v>44934</v>
@@ -4236,10 +4234,10 @@
     </row>
     <row r="272" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C272" s="5">
         <v>44934</v>

</xml_diff>